<commit_message>
Updated the basepage code   and added the scenarios in scenarios file
</commit_message>
<xml_diff>
--- a/target/classes/com/kw/scenarios/auto_scenarios.xlsx
+++ b/target/classes/com/kw/scenarios/auto_scenarios.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Test_step</t>
   </si>
@@ -60,9 +61,6 @@
     <t>enter password</t>
   </si>
   <si>
-    <t>mahadevia0</t>
-  </si>
-  <si>
     <t>click login button</t>
   </si>
   <si>
@@ -100,6 +98,45 @@
   </si>
   <si>
     <t>linkText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify the home page header </t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>isDisplayed</t>
+  </si>
+  <si>
+    <t>getText</t>
+  </si>
+  <si>
+    <t>//i18n-string[text()='User Guide']</t>
+  </si>
+  <si>
+    <t>get home page header title</t>
+  </si>
+  <si>
+    <t>//title</t>
+  </si>
+  <si>
+    <t>account-name</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>clickaccount name</t>
+  </si>
+  <si>
+    <t>signout</t>
+  </si>
+  <si>
+    <t>click signout link</t>
+  </si>
+  <si>
+    <t>M@hadevia0</t>
   </si>
 </sst>
 </file>
@@ -444,17 +481,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -464,10 +501,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -515,10 +552,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -532,30 +569,30 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
@@ -563,16 +600,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
@@ -580,50 +617,50 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>4</v>
@@ -631,26 +668,109 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>